<commit_message>
rearrange some files and folders, name it with more approriate name
</commit_message>
<xml_diff>
--- a/output/metrics_table.xlsx
+++ b/output/metrics_table.xlsx
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0288129956409292</v>
+        <v>0.02508122093216724</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1.754303205435584</v>
+        <v>1.528858312752999</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>-0.02255765456358594</v>
+        <v>-0.005335027006694312</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.007650090895285</v>
+        <v>2.054458368791535</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>122.2374456909146</v>
+        <v>125.2321712657749</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.174834153809177</v>
+        <v>1.577873015505964</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0288129956409292</v>
+        <v>0.02508122093216724</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.754303205435584</v>
+        <v>1.528858312752999</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>-0.02255765456358594</v>
+        <v>-0.005335027006694312</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2718816390986344</v>
+        <v>0.2310722898626279</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.30314809066396</v>
+        <v>1.103891934739909</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>-0.04263405241344964</v>
+        <v>-0.09264808326638718</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.179636079971869</v>
+        <v>1.07281325584755</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -609,7 +609,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>5.654079879722856</v>
+        <v>5.125105659861769</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>-0.1526999518359098</v>
+        <v>0.3029987632388947</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3184517083893237</v>
+        <v>0.3586701185774284</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1.526361754813724</v>
+        <v>1.71345967690549</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.2506362970891138</v>
+        <v>0.3171355525542741</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.849894658248598</v>
+        <v>2.926769900689424</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5.57260270679563</v>
+        <v>5.748028375001295</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -679,7 +679,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>2.799275969954425</v>
+        <v>2.895519011693499</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>25.57174180318244</v>
+        <v>27.8520716728664</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>50.00225435611976</v>
+        <v>54.70006311069905</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>25.27834912529596</v>
+        <v>27.48494852201295</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -725,7 +725,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2.849894658248598</v>
+        <v>2.926769900689424</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -733,7 +733,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>5.57260270679563</v>
+        <v>5.748028375001295</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>2.799275969954425</v>
+        <v>2.895519011693499</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5.558516966008419</v>
+        <v>5.390526155778248</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1.389629241502105</v>
+        <v>1.347631538944562</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>-5.364580107342256</v>
+        <v>-5.264481861280244</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -818,7 +818,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>6.205150644902133</v>
+        <v>6.205103218842413</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1.551287661225533</v>
+        <v>1.551275804710603</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>-6.205150604248047</v>
+        <v>-6.205103193010602</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
added tCan variable or leaf temperature or canopy temperature in the system, it already rewrite, so we can run the models with the combined models or not, then we also can implement the LT-1T-SDI12 in here, next step is to work on the firmware to send the leaf temperature measurements to the server
</commit_message>
<xml_diff>
--- a/output/metrics_table.xlsx
+++ b/output/metrics_table.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.783250203331104</v>
+        <v>0.168116600438055</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>30.05701886616807</v>
+        <v>12.67880533766137</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>-0.1080072224313204</v>
+        <v>-0.1668759703159332</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.422502990264492</v>
+        <v>2.207918313698289</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>131.337644740336</v>
+        <v>166.5139934301305</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2.114752798837253</v>
+        <v>1.491286757975844</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8211998537042153</v>
+        <v>0.1535421366873673</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>31.51332663650503</v>
+        <v>11.57964684698121</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>-0.07576361826579016</v>
+        <v>-0.1504373073101044</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3283468292454761</v>
+        <v>1.171562587402149</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.433143625711723</v>
+        <v>5.285493133634397</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>-0.2570599661905559</v>
+        <v>-1.13574721813202</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.027749466411331</v>
+        <v>2.017716160539228</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -609,7 +609,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4.485843825569138</v>
+        <v>9.102906687897267</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.6153910771011742</v>
+        <v>-1.659549614038649</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2813394282912318</v>
+        <v>1.1501706664674</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1.227969245944879</v>
+        <v>5.18898369194372</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.02797704810232221</v>
+        <v>-1.098814272880555</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.081821514029633</v>
+        <v>6.626071919176557</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1.965206940018132</v>
+        <v>12.97004535194824</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -679,7 +679,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.7846275087261094</v>
+        <v>6.546952104568479</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>37.99360091790392</v>
+        <v>46.37541056775313</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>69.01812104108224</v>
+        <v>90.77643370247736</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>36.79781281153418</v>
+        <v>46.25194408667794</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -725,7 +725,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.081821514029633</v>
+        <v>6.626071919176557</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -733,7 +733,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1.965206940018132</v>
+        <v>12.97004535194824</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.7846275087261094</v>
+        <v>6.546952104568479</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6.407986871359987</v>
+        <v>1.951511303086819</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -764,7 +764,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1.601264375955218</v>
+        <v>0.4878778257717046</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>-6.377598756348107</v>
+        <v>-1.945152282714844</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9.911997728903774</v>
+        <v>46.94930708714223</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2.476866631668696</v>
+        <v>11.73732677178556</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>-0.6699084001507262</v>
+        <v>40.25923679430914</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -818,7 +818,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>6.407986871359987</v>
+        <v>1.951511303086819</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1.601264375955218</v>
+        <v>0.4878778257717046</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -834,11 +834,104 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>-6.377598756348107</v>
+        <v>-1.945152282714844</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
           <t>ppm</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Leaf Temperature (NN)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1.237565324247811</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>5.772899471709905</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>-1.236618041992187</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Leaf Temperature (GL)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1.242150529272412</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>5.794288183194927</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>-0.7555795760566364</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Leaf Temperature (Combined)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.9028122187080343</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>°C</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>4.211368950241559</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>-0.6724491119384757</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>°C</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changed the folder and variables name from NN to DNN
</commit_message>
<xml_diff>
--- a/output/metrics_table.xlsx
+++ b/output/metrics_table.xlsx
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PAR (NN)</t>
+          <t>PAR (DNN)</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -566,7 +566,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Temperature (NN)</t>
+          <t>Temperature (DNN)</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -659,7 +659,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Humidity (NN)</t>
+          <t>Humidity (DNN)</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -752,7 +752,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CO2 (NN)</t>
+          <t>CO2 (DNN)</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -845,7 +845,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Leaf Temperature (NN)</t>
+          <t>Leaf Temperature (DNN)</t>
         </is>
       </c>
       <c r="B14" t="n">

</xml_diff>